<commit_message>
Make changes in time delay and robot working without stop
</commit_message>
<xml_diff>
--- a/ExcelOutputData/DataForIndeed.xlsx
+++ b/ExcelOutputData/DataForIndeed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects-UiPath\RPAAutomationFramework\ExcelOutputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F472960E-1F8F-417C-AA32-3C1988ACF2A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B050489-58DA-4F03-9A35-BE872890A217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="930" windowWidth="19740" windowHeight="9990" xr2:uid="{B9B83868-A3FE-4228-9C5A-A34FEFC3F149}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
   <si>
     <t>JobProfileName</t>
   </si>
@@ -50,43 +50,34 @@
     <t>DataQuest Corp</t>
   </si>
   <si>
-    <t>6 days ago</t>
-  </si>
-  <si>
-    <t>Application Developer: RPA</t>
-  </si>
-  <si>
-    <t>IBM 3.9</t>
-  </si>
-  <si>
-    <t>Today</t>
-  </si>
-  <si>
     <t>RPA Developer</t>
   </si>
   <si>
+    <t>Associate 2 - RPA Developer - Bangalore</t>
+  </si>
+  <si>
+    <t>KPMG 4.0</t>
+  </si>
+  <si>
+    <t>30+ days ago</t>
+  </si>
+  <si>
+    <t>Infosys technology limited 3.9</t>
+  </si>
+  <si>
+    <t>7 days ago</t>
+  </si>
+  <si>
     <t>Volvo Group 4.1</t>
   </si>
   <si>
-    <t>Associate 2 - RPA Developer - Bangalore</t>
-  </si>
-  <si>
-    <t>KPMG 4.0</t>
-  </si>
-  <si>
-    <t>30+ days ago</t>
-  </si>
-  <si>
     <t>UI Path &amp; RPA Developer</t>
   </si>
   <si>
     <t>Menorah Personnel Management India Private</t>
   </si>
   <si>
-    <t>19 days ago</t>
-  </si>
-  <si>
-    <t>Infosys technology limited 3.9</t>
+    <t>20 days ago</t>
   </si>
   <si>
     <t>Sr. RPA Developer</t>
@@ -95,22 +86,28 @@
     <t>Merck KGaA 4.0</t>
   </si>
   <si>
+    <t>Krish Tech Inc</t>
+  </si>
+  <si>
+    <t>25 days ago</t>
+  </si>
+  <si>
     <t>Capgemini 3.8</t>
   </si>
   <si>
-    <t>RPA Developer/ Senior Developer - Blue Prism</t>
-  </si>
-  <si>
-    <t>Dimension Data 3.8</t>
-  </si>
-  <si>
-    <t>RPA &amp; EPA SW Developer 3</t>
-  </si>
-  <si>
-    <t>Unisys 3.7</t>
-  </si>
-  <si>
-    <t>5 days ago</t>
+    <t>Looking for RPA Developers</t>
+  </si>
+  <si>
+    <t>Careator Technologies</t>
+  </si>
+  <si>
+    <t>Developer - RPA</t>
+  </si>
+  <si>
+    <t>Hudson's Bay Company 3.7</t>
+  </si>
+  <si>
+    <t>2 hours ago</t>
   </si>
 </sst>
 </file>
@@ -462,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D479125-8AC7-419F-9E7E-2B01875CD3B0}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -487,106 +484,216 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>